<commit_message>
revised pngs, reworking distance calculations
</commit_message>
<xml_diff>
--- a/src/main/TrainControllerSW/track_layout.xlsx
+++ b/src/main/TrainControllerSW/track_layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13477\Desktop\Github repos\ECE-1140\src\main\TrainControllerSW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E44E88-C4F3-4E81-BFB0-215AC33B2575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F36A500-F01A-4229-92B2-AE7310DADD75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -215,12 +215,6 @@
     <t>SWITCH (12-13; 1-13)</t>
   </si>
   <si>
-    <t>SWITCH TO YARD (57-yard)</t>
-  </si>
-  <si>
-    <t>SWITCH FROM YARD (Yard-63)</t>
-  </si>
-  <si>
     <t>SWITCH (76-77;77-101)</t>
   </si>
   <si>
@@ -228,9 +222,6 @@
   </si>
   <si>
     <t>SWITCH (85-86; 100-85)</t>
-  </si>
-  <si>
-    <t>SWITCH TO/FROM YARD (75-yard)</t>
   </si>
   <si>
     <t>SWITCH (15-16; 1-16)</t>
@@ -312,6 +303,15 @@
   </si>
   <si>
     <t>STATION; CENTRAL; UNDERGROUND</t>
+  </si>
+  <si>
+    <t>SWITCH TO YARD (57-YARD)</t>
+  </si>
+  <si>
+    <t>SWITCH FROM YARD (YARD-63)</t>
+  </si>
+  <si>
+    <t>SWITCH TO/FROM YARD (75-YARD)</t>
   </si>
 </sst>
 </file>
@@ -1661,7 +1661,7 @@
     </row>
     <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>8</v>
@@ -1803,7 +1803,7 @@
         <v>50</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="12">
@@ -1836,7 +1836,7 @@
         <v>50</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="12">
@@ -1962,7 +1962,7 @@
         <v>50</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="12">
@@ -1995,7 +1995,7 @@
         <v>50</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="12">
@@ -2121,7 +2121,7 @@
         <v>50</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="12">
@@ -2155,7 +2155,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="16" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2166,11 +2166,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L154"/>
+  <dimension ref="A1:M154"/>
   <sheetViews>
-    <sheetView zoomScale="78" workbookViewId="0">
+    <sheetView zoomScale="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G61" sqref="G61"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2188,7 +2188,7 @@
     <col min="14" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>11</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>36</v>
@@ -2220,8 +2220,10 @@
         <v>37</v>
       </c>
       <c r="K1" s="7"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -2250,7 +2252,7 @@
       </c>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="str">
         <f>A2</f>
         <v>Red</v>
@@ -2280,7 +2282,7 @@
       </c>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A70" si="1">A3</f>
         <v>Red</v>
@@ -2310,7 +2312,7 @@
       </c>
       <c r="L4" s="9"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2339,7 +2341,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2368,7 +2370,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2397,7 +2399,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2418,10 +2420,10 @@
         <v>40</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I8" s="12">
         <f t="shared" si="0"/>
@@ -2432,7 +2434,7 @@
         <v>4.125</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2461,7 +2463,7 @@
         <v>4.125</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2482,7 +2484,7 @@
         <v>40</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
       <c r="I10" s="12">
         <f t="shared" si="0"/>
@@ -2493,7 +2495,7 @@
         <v>4.125</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2522,7 +2524,7 @@
         <v>4.125</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2551,7 +2553,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2580,7 +2582,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2609,7 +2611,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2638,7 +2640,7 @@
         <v>0.85000000000000009</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2659,7 +2661,7 @@
         <v>40</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I16" s="12">
         <f t="shared" si="0"/>
@@ -2691,10 +2693,10 @@
         <v>40</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I17" s="12">
         <f t="shared" si="0"/>
@@ -2846,7 +2848,7 @@
         <v>55</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I22" s="12">
         <f t="shared" si="0"/>
@@ -2968,10 +2970,10 @@
         <v>70</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I26" s="12">
         <f t="shared" si="0"/>
@@ -3035,7 +3037,7 @@
         <v>70</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I28" s="12">
         <f t="shared" si="0"/>
@@ -3195,7 +3197,7 @@
         <v>70</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I33" s="12">
         <f t="shared" si="0"/>
@@ -3291,10 +3293,10 @@
         <v>70</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I36" s="12">
         <f t="shared" si="0"/>
@@ -3390,7 +3392,7 @@
         <v>70</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I39" s="12">
         <f t="shared" si="0"/>
@@ -3550,7 +3552,7 @@
         <v>70</v>
       </c>
       <c r="G44" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I44" s="12">
         <f t="shared" si="0"/>
@@ -3614,10 +3616,10 @@
         <v>70</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I46" s="12">
         <f t="shared" si="0"/>
@@ -3716,7 +3718,7 @@
         <v>38</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I49" s="12">
         <f t="shared" si="0"/>
@@ -3835,7 +3837,7 @@
         <v>55</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I53" s="12">
         <f t="shared" si="0"/>
@@ -4073,7 +4075,7 @@
         <v>39</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I61" s="12">
         <f t="shared" si="0"/>
@@ -5124,11 +5126,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L154"/>
+  <dimension ref="A1:N154"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D151" sqref="D151"/>
+    <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5146,7 +5148,7 @@
     <col min="14" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -5169,7 +5171,7 @@
         <v>11</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>36</v>
@@ -5178,10 +5180,13 @@
         <v>37</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -5213,7 +5218,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="str">
         <f>A2</f>
         <v>Green</v>
@@ -5237,7 +5242,7 @@
         <v>47</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I3" s="3">
         <f t="shared" ref="I3:I66" si="1">E3*D3/100</f>
@@ -5252,7 +5257,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A70" si="2">A3</f>
         <v>Green</v>
@@ -5286,7 +5291,7 @@
       </c>
       <c r="L4" s="9"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5319,7 +5324,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5352,7 +5357,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5385,7 +5390,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5419,7 +5424,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5452,7 +5457,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5476,7 +5481,7 @@
         <v>48</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I10" s="3">
         <f t="shared" si="1"/>
@@ -5491,7 +5496,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5524,7 +5529,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5557,7 +5562,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5593,7 +5598,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5626,7 +5631,7 @@
         <v>7.7142857142857153</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5659,7 +5664,7 @@
         <v>7.7142857142857153</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -5716,7 +5721,7 @@
         <v>22</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I17" s="3">
         <f t="shared" si="1"/>
@@ -5923,7 +5928,7 @@
         <v>49</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I23" s="3">
         <f t="shared" si="1"/>
@@ -6157,7 +6162,7 @@
         <v>30</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I30" s="3">
         <f t="shared" si="1"/>
@@ -6229,7 +6234,7 @@
         <v>50</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I32" s="3">
         <f t="shared" si="1"/>
@@ -6505,10 +6510,10 @@
         <v>30</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I40" s="3">
         <f t="shared" si="1"/>
@@ -6835,7 +6840,7 @@
         <v>53</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I49" s="3">
         <f t="shared" si="1"/>
@@ -7162,7 +7167,7 @@
         <v>54</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I58" s="3">
         <f t="shared" si="1"/>
@@ -7198,7 +7203,7 @@
         <v>30</v>
       </c>
       <c r="G59" s="11" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="I59" s="3">
         <f t="shared" si="1"/>
@@ -7333,7 +7338,7 @@
         <v>30</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="I63" s="3">
         <f t="shared" si="1"/>
@@ -7435,10 +7440,10 @@
         <v>70</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I66" s="3">
         <f t="shared" si="1"/>
@@ -7708,7 +7713,7 @@
         <v>51</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I74" s="3">
         <f t="shared" si="5"/>
@@ -7810,7 +7815,7 @@
         <v>40</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I77" s="3">
         <f t="shared" si="5"/>
@@ -7846,10 +7851,10 @@
         <v>70</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I78" s="3">
         <f t="shared" ref="I78:I109" si="8">E78*D78/100</f>
@@ -8116,7 +8121,7 @@
         <v>70</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I86" s="3">
         <f t="shared" si="8"/>
@@ -8221,7 +8226,7 @@
         <v>52</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I89" s="3">
         <f t="shared" si="8"/>
@@ -8488,10 +8493,10 @@
         <v>25</v>
       </c>
       <c r="G97" s="11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H97" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I97" s="3">
         <f t="shared" si="8"/>
@@ -8795,7 +8800,7 @@
         <v>STATION; DORMONT</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I106" s="3">
         <f t="shared" si="8"/>
@@ -9100,7 +9105,7 @@
         <v>STATION; GLENBURY (First)</v>
       </c>
       <c r="H115" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I115" s="3">
         <f t="shared" si="10"/>
@@ -9407,7 +9412,7 @@
         <v>STATION; OVERBROOK; UNDERGROUND</v>
       </c>
       <c r="H124" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I124" s="3">
         <f t="shared" si="10"/>
@@ -9735,7 +9740,7 @@
         <v>STATION; INGLEWOOD; UNDERGROUND</v>
       </c>
       <c r="H133" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I133" s="3">
         <f t="shared" si="10"/>
@@ -10063,7 +10068,7 @@
         <v>STATION; CENTRAL; UNDERGROUND</v>
       </c>
       <c r="H142" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I142" s="3">
         <f t="shared" si="10"/>

</xml_diff>